<commit_message>
improve aesthetics of generated excel reports and integration with backend
</commit_message>
<xml_diff>
--- a/analizing_data/filled_reports/form1_report.xlsx
+++ b/analizing_data/filled_reports/form1_report.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Отчет проверки" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,15 +26,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <i val="1"/>
+      <sz val="9"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D3D3D3"/>
+        <bgColor rgb="00D3D3D3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,9 +82,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -425,463 +476,567 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="8" customWidth="1" min="1" max="1"/>
+    <col width="60" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="40" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Редакция от 03.10.2025</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>УПП</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Дата проведения проверки</t>
-        </is>
-      </c>
-    </row>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>Дата проведения проверки:</t>
+        </is>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4"/>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="4" t="inlineStr">
         <is>
           <t>Чек-лист оценки состояния оборудования и рабочего пространства рабочего персонала</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="5" t="inlineStr">
         <is>
           <t>№ п/п</t>
         </is>
       </c>
-      <c r="B6" s="1" t="inlineStr">
+      <c r="B6" s="6" t="inlineStr">
         <is>
           <t>Критерий оценки</t>
         </is>
       </c>
-      <c r="C6" s="1" t="inlineStr">
+      <c r="C6" s="5" t="inlineStr">
         <is>
           <t>Оценка</t>
         </is>
       </c>
-      <c r="D6" s="1" t="inlineStr"/>
-      <c r="E6" s="1" t="inlineStr">
+      <c r="D6" s="5" t="inlineStr"/>
+      <c r="E6" s="6" t="inlineStr">
         <is>
           <t>Краткий комментарий с указанием номера единицы оборудования, где выявлено несоответствие, и фото несоответствия</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n"/>
-      <c r="B7" s="1" t="n"/>
-      <c r="C7" s="1" t="inlineStr">
+      <c r="A7" s="5" t="n"/>
+      <c r="B7" s="5" t="n"/>
+      <c r="C7" s="5" t="inlineStr">
         <is>
           <t>соответствует</t>
         </is>
       </c>
-      <c r="D7" s="1" t="inlineStr">
+      <c r="D7" s="5" t="inlineStr">
         <is>
           <t>не соответствует</t>
         </is>
       </c>
-      <c r="E7" s="1" t="n"/>
+      <c r="E7" s="5" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="7" t="inlineStr">
         <is>
           <t>А</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="8" t="inlineStr">
         <is>
           <t>Состояние рабочего пространства укладчика-упаковщика (оператора ЦП, наладчика участка производства СКПГ, дробильщика, подсобного рабочего)</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="8" t="inlineStr">
         <is>
           <t>На полу отсутствует пыль, грязь. Под оборудованием и вокруг него отсутствует россыпи сырья и/или красителя, мусор, литники, продукция, пакеты из-под материала, другие предметы</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="8" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="8" t="inlineStr">
         <is>
           <t>Личные вещи отсутствуют в рабочей зоне работника (на оборудовании, стуле, стойке и т.д.), в том числе спецодежда.</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="8" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="8" t="inlineStr">
         <is>
           <t>На оборудовании и в рабочей зоне отсутствуют посторонние предметы, непредназначенные для выполнения профессиональных обязанностей</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="8" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="8" t="inlineStr">
         <is>
           <t>Уборочный инвентарь имеется в наличии и размещен аккуратно в установленном месте</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="8" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="8" t="inlineStr">
         <is>
           <t>Тара, упаковочные материалы, поддоны, готовая продукция, несоответствующая продукция находятся в зонах разметки согласно стандарту идеального рабочего места, размещенному на оборудовании</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="8" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="8" t="inlineStr">
         <is>
           <t>Проходы вокруг оборудования свободные и нет загромождений продукцией, тарой, поддонами и другими предметами</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
+      <c r="C14" s="7" t="inlineStr"/>
+      <c r="D14" s="7" t="inlineStr"/>
+      <c r="E14" s="8" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="8" t="inlineStr">
         <is>
           <t>Общий балл за раздел А</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" s="7" t="n">
         <v>0</v>
       </c>
     </row>
+    <row r="16"/>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="7" t="inlineStr">
         <is>
           <t>В</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="8" t="inlineStr">
         <is>
           <t>Состояние оборудования</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="7" t="inlineStr">
         <is>
           <t>В1</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="8" t="inlineStr">
         <is>
           <t>Ответственность наладчика производственного участка</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="8" t="inlineStr">
         <is>
           <t>Отсутствие пыли и грязи на оборудовании (станине, конвейерной ленте, шлангах и других элементах оборудования) 1</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
+      <c r="C19" s="7" t="inlineStr"/>
+      <c r="D19" s="7" t="inlineStr"/>
+      <c r="E19" s="8" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" s="8" t="inlineStr">
         <is>
           <t>Тумбочки и шкафы с инструментами наладчиков идентифицированы и чистые.</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
+      <c r="C20" s="7" t="inlineStr"/>
+      <c r="D20" s="7" t="inlineStr"/>
+      <c r="E20" s="8" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="8" t="inlineStr">
         <is>
           <t>На оборудовании имеются все защитные экраны.</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
+      <c r="C21" s="7" t="inlineStr"/>
+      <c r="D21" s="7" t="inlineStr"/>
+      <c r="E21" s="8" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="8" t="inlineStr">
         <is>
           <t>На оборудовании отсутствуют крепления скотчем, картона на конвейерной ленте и других элементах оборудования</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
+      <c r="C22" s="7" t="inlineStr"/>
+      <c r="D22" s="7" t="inlineStr"/>
+      <c r="E22" s="8" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="n">
+      <c r="A23" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" s="8" t="inlineStr">
         <is>
           <t>Внутри оборудования отсутствуют посторонние предметы, в том числе остатки продукции от прошлых производственных партий и текущей производственной партии.</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
+      <c r="C23" s="7" t="inlineStr"/>
+      <c r="D23" s="7" t="inlineStr"/>
+      <c r="E23" s="8" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="n">
+      <c r="A24" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="8" t="inlineStr">
         <is>
           <t>Технологическая оснастка (пресс-формы) хранятся в специально отведенных местах.</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
+      <c r="C24" s="7" t="inlineStr"/>
+      <c r="D24" s="7" t="inlineStr"/>
+      <c r="E24" s="8" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Общий балл за раздел В1</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
+      <c r="B25" s="8" t="inlineStr">
+        <is>
+          <t>Общий балл за подраздел В1</t>
+        </is>
+      </c>
+      <c r="C25" s="7" t="n">
         <v>0</v>
       </c>
     </row>
+    <row r="26"/>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="7" t="inlineStr">
         <is>
           <t>В2</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" s="8" t="inlineStr">
         <is>
           <t>Ответственность персонала ЭМО</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
+      <c r="A28" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="8" t="inlineStr">
         <is>
           <t>Течь масла, охлаждающих жидкостей с оборудования отсутствует. Пол около оборудования чистый и сухой</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
+      <c r="C28" s="7" t="inlineStr"/>
+      <c r="D28" s="7" t="inlineStr"/>
+      <c r="E28" s="8" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" t="n">
+      <c r="A29" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" s="8" t="inlineStr">
         <is>
           <t>Внутри оборудования все элементы (провода, шланги, и др.) закреплены монтажными стяжками (применение скотча, целлофана, ленточек, ветоши и др. посторонних предметов исключено).</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
+      <c r="C29" s="7" t="inlineStr"/>
+      <c r="D29" s="7" t="inlineStr"/>
+      <c r="E29" s="8" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" t="n">
+      <c r="A30" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" s="8" t="inlineStr">
         <is>
           <t>На технологическом оборудовании и других видах оборудования, применяемых на участке, отсутствуют повреждения изоляции электропроводки, лакокрасочных покрытий и т.д.</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr"/>
+      <c r="C30" s="7" t="inlineStr"/>
+      <c r="D30" s="7" t="inlineStr"/>
+      <c r="E30" s="8" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" t="n">
+      <c r="A31" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" s="8" t="inlineStr">
         <is>
           <t>Отсутствуют вещи, оставшиеся после работы вспомогательных служб на производственном участке</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr"/>
+      <c r="C31" s="7" t="inlineStr"/>
+      <c r="D31" s="7" t="inlineStr"/>
+      <c r="E31" s="8" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" t="n">
+      <c r="A32" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" s="8" t="inlineStr">
         <is>
           <t>Панель управления в технически исправном состоянии, все надписи читаемы, видимые повреждения отсутствуют</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr"/>
+      <c r="C32" s="7" t="inlineStr"/>
+      <c r="D32" s="7" t="inlineStr"/>
+      <c r="E32" s="8" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" t="n">
+      <c r="A33" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" s="8" t="inlineStr">
         <is>
           <t>На оборудовании имеются все защитные ограждения, предусмотренные конструкцией оборудования, в том числе закрывающие подвижные механизмы. Критерий оценки Оценка Краткий комментарий с указанием номера единицы оборудования, где выявлено несоответствие, и фото несоответствия не соответствует</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr"/>
+      <c r="C33" s="7" t="inlineStr"/>
+      <c r="D33" s="7" t="inlineStr"/>
+      <c r="E33" s="8" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Общий балл за раздел В2</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
+      <c r="B34" s="8" t="inlineStr">
+        <is>
+          <t>Общий балл за подраздел В2</t>
+        </is>
+      </c>
+      <c r="C34" s="7" t="n">
         <v>0</v>
       </c>
     </row>
+    <row r="35"/>
     <row r="36">
-      <c r="B36" t="inlineStr">
+      <c r="B36" s="8" t="inlineStr">
         <is>
           <t>Общий балл за раздел В</t>
         </is>
       </c>
-      <c r="C36" t="n">
+      <c r="C36" s="7" t="n">
         <v>0</v>
       </c>
     </row>
+    <row r="37"/>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="7" t="inlineStr">
         <is>
           <t>С</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" s="8" t="inlineStr">
         <is>
           <t>Состояние производственного участка и вспомогательных помещений (кладовых, складов)</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
+      <c r="A39" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" s="8" t="inlineStr">
         <is>
           <t>Пол, подоконники, колонны, стены, двери чистые (нет пыли, грязи и др.) и не имеют повреждений</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr"/>
+      <c r="C39" s="7" t="inlineStr"/>
+      <c r="D39" s="7" t="inlineStr"/>
+      <c r="E39" s="8" t="inlineStr"/>
     </row>
     <row r="40">
-      <c r="A40" t="n">
+      <c r="A40" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" s="8" t="inlineStr">
         <is>
           <t>Все отходы собираются раздельно.</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr"/>
+      <c r="C40" s="7" t="inlineStr"/>
+      <c r="D40" s="7" t="inlineStr"/>
+      <c r="E40" s="8" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="A41" t="n">
+      <c r="A41" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" s="8" t="inlineStr">
         <is>
           <t>Места и стеллажи, предназначенные для хранения сырья, основных и вспомогательных материалов (на участке, кладовых, складах) идентифицированы и в исправном состоянии.</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr"/>
+      <c r="C41" s="7" t="inlineStr"/>
+      <c r="D41" s="7" t="inlineStr"/>
+      <c r="E41" s="8" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" t="n">
+      <c r="A42" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="8" t="inlineStr">
         <is>
           <t>В маркировочных ярлыках (этикетках) для идентификации изготавливаемой продукции, размещенных на оборудовании в ячейках с надписью «Для маркировочных ярлыков», указана дата, соответствующая дню проведения проверки</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr"/>
+      <c r="C42" s="7" t="inlineStr"/>
+      <c r="D42" s="7" t="inlineStr"/>
+      <c r="E42" s="8" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" t="n">
+      <c r="A43" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" s="8" t="inlineStr">
         <is>
           <t>Электроштабелеры, гидротележеки размещены в установленных местах, идентифицированы наименованием участка и имеют отметку о последних испытаниях</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr"/>
+      <c r="C43" s="7" t="inlineStr"/>
+      <c r="D43" s="7" t="inlineStr"/>
+      <c r="E43" s="8" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="A44" t="n">
+      <c r="A44" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B44" s="8" t="inlineStr">
         <is>
           <t>Место размещения на участке питьевой воды содержится в надлежащем состоянии: бутыль с водой без упаковочных материалов, использованные стаканчики в урне, посторонних предметов на кулере и около него нет, урна не переполнена</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr"/>
+      <c r="C44" s="7" t="inlineStr"/>
+      <c r="D44" s="7" t="inlineStr"/>
+      <c r="E44" s="8" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="B45" t="inlineStr">
+      <c r="B45" s="8" t="inlineStr">
         <is>
           <t>Общий балл за раздел С</t>
         </is>
       </c>
-      <c r="C45" t="n">
+      <c r="C45" s="7" t="n">
         <v>0</v>
       </c>
     </row>
+    <row r="46"/>
     <row r="47">
-      <c r="B47" t="inlineStr">
+      <c r="B47" s="9" t="inlineStr">
         <is>
           <t>Итоговая оценка структурному подразделению</t>
         </is>
       </c>
-      <c r="C47" t="n">
+      <c r="E47" s="8" t="n">
         <v>0</v>
       </c>
     </row>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50" ht="25" customHeight="1">
+      <c r="A50" s="7" t="inlineStr">
+        <is>
+          <t>Проверку проводил _____________________ ______________ _______________________</t>
+        </is>
+      </c>
+      <c r="B50" s="10" t="n"/>
+      <c r="C50" s="10" t="n"/>
+      <c r="D50" s="10" t="n"/>
+      <c r="E50" s="10" t="n"/>
+    </row>
+    <row r="51" ht="25" customHeight="1">
+      <c r="A51" s="7" t="inlineStr">
+        <is>
+          <t>должность подпись расшифровка подпись</t>
+        </is>
+      </c>
+      <c r="B51" s="10" t="n"/>
+      <c r="C51" s="10" t="n"/>
+      <c r="D51" s="10" t="n"/>
+      <c r="E51" s="10" t="n"/>
+    </row>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54" ht="60" customHeight="1">
+      <c r="A54" s="11" t="inlineStr">
+        <is>
+          <t>* Итоговая оценка структурному подразделению проставляется проверяющим при выявлении одного и того же несоответствия 2 раза в размере «3 балла», при выявлении одного и того же несоответствия более 2 раз - «2 балла». При отсутствии повторяющихся несоответствий в ходе проведения проверки данная графа проверяющим не заполняется.</t>
+        </is>
+      </c>
+    </row>
+    <row r="55"/>
+    <row r="56"/>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A54:E56"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="B47:D47"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add violation report with images
</commit_message>
<xml_diff>
--- a/analizing_data/filled_reports/form1_report.xlsx
+++ b/analizing_data/filled_reports/form1_report.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -35,10 +35,6 @@
     <font>
       <b val="1"/>
       <sz val="12"/>
-    </font>
-    <font>
-      <i val="1"/>
-      <sz val="9"/>
     </font>
     <font>
       <b val="1"/>
@@ -82,7 +78,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -90,10 +86,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -107,9 +103,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,14 +487,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Редакция от 03.10.2025</t>
+          <t>Редакция от 2024-01-15</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>УПП</t>
+          <t>Производственный цех №1</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -509,8 +502,19 @@
           <t>Дата проведения проверки:</t>
         </is>
       </c>
-    </row>
-    <row r="3"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2024-01-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>Проверяющий: Иванов А.С.</t>
+        </is>
+      </c>
+    </row>
     <row r="4"/>
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
@@ -560,482 +564,211 @@
     <row r="8">
       <c r="A8" s="7" t="inlineStr">
         <is>
-          <t>А</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B8" s="8" t="inlineStr">
         <is>
-          <t>Состояние рабочего пространства укладчика-упаковщика (оператора ЦП, наладчика участка производства СКПГ, дробильщика, подсобного рабочего)</t>
+          <t>Организация рабочего места</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="n">
-        <v>1</v>
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
       </c>
       <c r="B9" s="8" t="inlineStr">
         <is>
-          <t>На полу отсутствует пыль, грязь. Под оборудованием и вокруг него отсутствует россыпи сырья и/или красителя, мусор, литники, продукция, пакеты из-под материала, другие предметы</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="inlineStr"/>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="8" t="inlineStr"/>
+          <t>Рабочий стол</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="8" t="inlineStr">
         <is>
-          <t>Личные вещи отсутствуют в рабочей зоне работника (на оборудовании, стуле, стойке и т.д.), в том числе спецодежда.</t>
+          <t>Стол чистый, без посторонних предметов</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr"/>
-      <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="8" t="inlineStr"/>
+      <c r="D10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8" t="inlineStr">
+        <is>
+          <t>На столе обнаружены инструменты не по назначению</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" s="8" t="inlineStr">
         <is>
-          <t>На оборудовании и в рабочей зоне отсутствуют посторонние предметы, непредназначенные для выполнения профессиональных обязанностей</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="inlineStr"/>
+          <t>Поверхность стола без повреждений</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="8" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B12" s="8" t="inlineStr">
-        <is>
-          <t>Уборочный инвентарь имеется в наличии и размещен аккуратно в установленном месте</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="inlineStr"/>
-      <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="8" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B13" s="8" t="inlineStr">
-        <is>
-          <t>Тара, упаковочные материалы, поддоны, готовая продукция, несоответствующая продукция находятся в зонах разметки согласно стандарту идеального рабочего места, размещенному на оборудовании</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="inlineStr"/>
-      <c r="D13" s="7" t="inlineStr"/>
-      <c r="E13" s="8" t="inlineStr"/>
-    </row>
+      <c r="B12" s="9" t="inlineStr">
+        <is>
+          <t>Общий балл за подраздел A1</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13"/>
     <row r="14">
-      <c r="A14" s="7" t="n">
-        <v>6</v>
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
       </c>
       <c r="B14" s="8" t="inlineStr">
         <is>
-          <t>Проходы вокруг оборудования свободные и нет загромождений продукцией, тарой, поддонами и другими предметами</t>
-        </is>
-      </c>
-      <c r="C14" s="7" t="inlineStr"/>
-      <c r="D14" s="7" t="inlineStr"/>
-      <c r="E14" s="8" t="inlineStr"/>
+          <t>Оборудование</t>
+        </is>
+      </c>
     </row>
     <row r="15">
+      <c r="A15" s="7" t="n">
+        <v>3</v>
+      </c>
       <c r="B15" s="8" t="inlineStr">
         <is>
-          <t>Общий балл за раздел А</t>
-        </is>
-      </c>
-      <c r="C15" s="7" t="n">
+          <t>Оборудование исправно</t>
+        </is>
+      </c>
+      <c r="C15" s="7" t="inlineStr"/>
+      <c r="D15" s="7" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="16"/>
-    <row r="17">
-      <c r="A17" s="7" t="inlineStr">
-        <is>
-          <t>В</t>
-        </is>
-      </c>
-      <c r="B17" s="8" t="inlineStr">
-        <is>
-          <t>Состояние оборудования</t>
-        </is>
-      </c>
-    </row>
+      <c r="E15" s="8" t="inlineStr">
+        <is>
+          <t>Станок №5 требует регулировки</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="9" t="inlineStr">
+        <is>
+          <t>Общий балл за подраздел A2</t>
+        </is>
+      </c>
+      <c r="C16" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17"/>
     <row r="18">
-      <c r="A18" s="7" t="inlineStr">
-        <is>
-          <t>В1</t>
-        </is>
-      </c>
-      <c r="B18" s="8" t="inlineStr">
-        <is>
-          <t>Ответственность наладчика производственного участка</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="7" t="n">
+      <c r="B18" s="9" t="inlineStr">
+        <is>
+          <t>Общий балл за раздел A</t>
+        </is>
+      </c>
+      <c r="C18" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B19" s="8" t="inlineStr">
-        <is>
-          <t>Отсутствие пыли и грязи на оборудовании (станине, конвейерной ленте, шлангах и других элементах оборудования) 1</t>
-        </is>
-      </c>
-      <c r="C19" s="7" t="inlineStr"/>
-      <c r="D19" s="7" t="inlineStr"/>
-      <c r="E19" s="8" t="inlineStr"/>
-    </row>
+    </row>
+    <row r="19"/>
     <row r="20">
-      <c r="A20" s="7" t="n">
-        <v>2</v>
+      <c r="A20" s="7" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
       </c>
       <c r="B20" s="8" t="inlineStr">
         <is>
-          <t>Тумбочки и шкафы с инструментами наладчиков идентифицированы и чистые.</t>
-        </is>
-      </c>
-      <c r="C20" s="7" t="inlineStr"/>
-      <c r="D20" s="7" t="inlineStr"/>
-      <c r="E20" s="8" t="inlineStr"/>
+          <t>Средства индивидуальной защиты</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B21" s="8" t="inlineStr">
         <is>
-          <t>На оборудовании имеются все защитные экраны.</t>
+          <t>Каска надета правильно</t>
         </is>
       </c>
       <c r="C21" s="7" t="inlineStr"/>
-      <c r="D21" s="7" t="inlineStr"/>
-      <c r="E21" s="8" t="inlineStr"/>
+      <c r="D21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="8" t="inlineStr">
+        <is>
+          <t>Рабочий Петров И.С. без каски</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B22" s="8" t="inlineStr">
         <is>
-          <t>На оборудовании отсутствуют крепления скотчем, картона на конвейерной ленте и других элементах оборудования</t>
-        </is>
-      </c>
-      <c r="C22" s="7" t="inlineStr"/>
+          <t>Перчатки соответствуют требованиям</t>
+        </is>
+      </c>
+      <c r="C22" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="D22" s="7" t="inlineStr"/>
       <c r="E22" s="8" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B23" s="8" t="inlineStr">
-        <is>
-          <t>Внутри оборудования отсутствуют посторонние предметы, в том числе остатки продукции от прошлых производственных партий и текущей производственной партии.</t>
-        </is>
-      </c>
-      <c r="C23" s="7" t="inlineStr"/>
-      <c r="D23" s="7" t="inlineStr"/>
-      <c r="E23" s="8" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B24" s="8" t="inlineStr">
-        <is>
-          <t>Технологическая оснастка (пресс-формы) хранятся в специально отведенных местах.</t>
-        </is>
-      </c>
-      <c r="C24" s="7" t="inlineStr"/>
-      <c r="D24" s="7" t="inlineStr"/>
-      <c r="E24" s="8" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="B25" s="8" t="inlineStr">
-        <is>
-          <t>Общий балл за подраздел В1</t>
-        </is>
-      </c>
-      <c r="C25" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
+      <c r="B23" s="9" t="inlineStr">
+        <is>
+          <t>Общий балл за раздел B</t>
+        </is>
+      </c>
+      <c r="C23" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24"/>
+    <row r="25"/>
     <row r="26"/>
-    <row r="27">
+    <row r="27" ht="25" customHeight="1">
       <c r="A27" s="7" t="inlineStr">
         <is>
-          <t>В2</t>
-        </is>
-      </c>
-      <c r="B27" s="8" t="inlineStr">
-        <is>
-          <t>Ответственность персонала ЭМО</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B28" s="8" t="inlineStr">
-        <is>
-          <t>Течь масла, охлаждающих жидкостей с оборудования отсутствует. Пол около оборудования чистый и сухой</t>
-        </is>
-      </c>
-      <c r="C28" s="7" t="inlineStr"/>
-      <c r="D28" s="7" t="inlineStr"/>
-      <c r="E28" s="8" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B29" s="8" t="inlineStr">
-        <is>
-          <t>Внутри оборудования все элементы (провода, шланги, и др.) закреплены монтажными стяжками (применение скотча, целлофана, ленточек, ветоши и др. посторонних предметов исключено).</t>
-        </is>
-      </c>
-      <c r="C29" s="7" t="inlineStr"/>
-      <c r="D29" s="7" t="inlineStr"/>
-      <c r="E29" s="8" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B30" s="8" t="inlineStr">
-        <is>
-          <t>На технологическом оборудовании и других видах оборудования, применяемых на участке, отсутствуют повреждения изоляции электропроводки, лакокрасочных покрытий и т.д.</t>
-        </is>
-      </c>
-      <c r="C30" s="7" t="inlineStr"/>
-      <c r="D30" s="7" t="inlineStr"/>
-      <c r="E30" s="8" t="inlineStr"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B31" s="8" t="inlineStr">
-        <is>
-          <t>Отсутствуют вещи, оставшиеся после работы вспомогательных служб на производственном участке</t>
-        </is>
-      </c>
-      <c r="C31" s="7" t="inlineStr"/>
-      <c r="D31" s="7" t="inlineStr"/>
-      <c r="E31" s="8" t="inlineStr"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B32" s="8" t="inlineStr">
-        <is>
-          <t>Панель управления в технически исправном состоянии, все надписи читаемы, видимые повреждения отсутствуют</t>
-        </is>
-      </c>
-      <c r="C32" s="7" t="inlineStr"/>
-      <c r="D32" s="7" t="inlineStr"/>
-      <c r="E32" s="8" t="inlineStr"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B33" s="8" t="inlineStr">
-        <is>
-          <t>На оборудовании имеются все защитные ограждения, предусмотренные конструкцией оборудования, в том числе закрывающие подвижные механизмы. Критерий оценки Оценка Краткий комментарий с указанием номера единицы оборудования, где выявлено несоответствие, и фото несоответствия не соответствует</t>
-        </is>
-      </c>
-      <c r="C33" s="7" t="inlineStr"/>
-      <c r="D33" s="7" t="inlineStr"/>
-      <c r="E33" s="8" t="inlineStr"/>
-    </row>
-    <row r="34">
-      <c r="B34" s="8" t="inlineStr">
-        <is>
-          <t>Общий балл за подраздел В2</t>
-        </is>
-      </c>
-      <c r="C34" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35"/>
-    <row r="36">
-      <c r="B36" s="8" t="inlineStr">
-        <is>
-          <t>Общий балл за раздел В</t>
-        </is>
-      </c>
-      <c r="C36" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37"/>
-    <row r="38">
-      <c r="A38" s="7" t="inlineStr">
-        <is>
-          <t>С</t>
-        </is>
-      </c>
-      <c r="B38" s="8" t="inlineStr">
-        <is>
-          <t>Состояние производственного участка и вспомогательных помещений (кладовых, складов)</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B39" s="8" t="inlineStr">
-        <is>
-          <t>Пол, подоконники, колонны, стены, двери чистые (нет пыли, грязи и др.) и не имеют повреждений</t>
-        </is>
-      </c>
-      <c r="C39" s="7" t="inlineStr"/>
-      <c r="D39" s="7" t="inlineStr"/>
-      <c r="E39" s="8" t="inlineStr"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B40" s="8" t="inlineStr">
-        <is>
-          <t>Все отходы собираются раздельно.</t>
-        </is>
-      </c>
-      <c r="C40" s="7" t="inlineStr"/>
-      <c r="D40" s="7" t="inlineStr"/>
-      <c r="E40" s="8" t="inlineStr"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B41" s="8" t="inlineStr">
-        <is>
-          <t>Места и стеллажи, предназначенные для хранения сырья, основных и вспомогательных материалов (на участке, кладовых, складах) идентифицированы и в исправном состоянии.</t>
-        </is>
-      </c>
-      <c r="C41" s="7" t="inlineStr"/>
-      <c r="D41" s="7" t="inlineStr"/>
-      <c r="E41" s="8" t="inlineStr"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B42" s="8" t="inlineStr">
-        <is>
-          <t>В маркировочных ярлыках (этикетках) для идентификации изготавливаемой продукции, размещенных на оборудовании в ячейках с надписью «Для маркировочных ярлыков», указана дата, соответствующая дню проведения проверки</t>
-        </is>
-      </c>
-      <c r="C42" s="7" t="inlineStr"/>
-      <c r="D42" s="7" t="inlineStr"/>
-      <c r="E42" s="8" t="inlineStr"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B43" s="8" t="inlineStr">
-        <is>
-          <t>Электроштабелеры, гидротележеки размещены в установленных местах, идентифицированы наименованием участка и имеют отметку о последних испытаниях</t>
-        </is>
-      </c>
-      <c r="C43" s="7" t="inlineStr"/>
-      <c r="D43" s="7" t="inlineStr"/>
-      <c r="E43" s="8" t="inlineStr"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B44" s="8" t="inlineStr">
-        <is>
-          <t>Место размещения на участке питьевой воды содержится в надлежащем состоянии: бутыль с водой без упаковочных материалов, использованные стаканчики в урне, посторонних предметов на кулере и около него нет, урна не переполнена</t>
-        </is>
-      </c>
-      <c r="C44" s="7" t="inlineStr"/>
-      <c r="D44" s="7" t="inlineStr"/>
-      <c r="E44" s="8" t="inlineStr"/>
-    </row>
-    <row r="45">
-      <c r="B45" s="8" t="inlineStr">
-        <is>
-          <t>Общий балл за раздел С</t>
-        </is>
-      </c>
-      <c r="C45" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46"/>
-    <row r="47">
-      <c r="B47" s="9" t="inlineStr">
-        <is>
-          <t>Итоговая оценка структурному подразделению</t>
-        </is>
-      </c>
-      <c r="E47" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50" ht="25" customHeight="1">
-      <c r="A50" s="7" t="inlineStr">
-        <is>
           <t>Проверку проводил _____________________ ______________ _______________________</t>
         </is>
       </c>
-      <c r="B50" s="10" t="n"/>
-      <c r="C50" s="10" t="n"/>
-      <c r="D50" s="10" t="n"/>
-      <c r="E50" s="10" t="n"/>
-    </row>
-    <row r="51" ht="25" customHeight="1">
-      <c r="A51" s="7" t="inlineStr">
+      <c r="B27" s="10" t="n"/>
+      <c r="C27" s="10" t="n"/>
+      <c r="D27" s="10" t="n"/>
+      <c r="E27" s="10" t="n"/>
+    </row>
+    <row r="28" ht="25" customHeight="1">
+      <c r="A28" s="7" t="inlineStr">
         <is>
           <t>должность подпись расшифровка подпись</t>
         </is>
       </c>
-      <c r="B51" s="10" t="n"/>
-      <c r="C51" s="10" t="n"/>
-      <c r="D51" s="10" t="n"/>
-      <c r="E51" s="10" t="n"/>
-    </row>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54" ht="60" customHeight="1">
-      <c r="A54" s="11" t="inlineStr">
-        <is>
-          <t>* Итоговая оценка структурному подразделению проставляется проверяющим при выявлении одного и того же несоответствия 2 раза в размере «3 балла», при выявлении одного и того же несоответствия более 2 раз - «2 балла». При отсутствии повторяющихся несоответствий в ходе проведения проверки данная графа проверяющим не заполняется.</t>
-        </is>
-      </c>
-    </row>
-    <row r="55"/>
-    <row r="56"/>
+      <c r="B28" s="10" t="n"/>
+      <c r="C28" s="10" t="n"/>
+      <c r="D28" s="10" t="n"/>
+      <c r="E28" s="10" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="A54:E56"/>
-    <mergeCell ref="A51:E51"/>
+  <mergeCells count="3">
     <mergeCell ref="A5:E5"/>
-    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A27:E27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>